<commit_message>
modified extent report code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ActitimeHybridFramework_TestData.xlsx
+++ b/src/test/resources/TestData/ActitimeHybridFramework_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52861E70-C888-4AE3-9FC9-F2E1BDD16F8A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7470EFFE-AF8E-47FA-BFAF-CEE604B92579}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>colunm Name 1</t>
-  </si>
-  <si>
-    <t>colunm Name 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>galatpassword</t>
+  </si>
+  <si>
+    <t>rajmitra</t>
+  </si>
+  <si>
+    <t>manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -61,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,23 +367,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upated location for Excel Data sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ActitimeHybridFramework_TestData.xlsx
+++ b/src/test/resources/TestData/ActitimeHybridFramework_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D935CD3F-1CC8-455B-9BAC-1AE885C04DDF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F787BD42-EC8F-4594-A3BD-AF7B4A4F94B0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>